<commit_message>
add function to generate exams and solutions
</commit_message>
<xml_diff>
--- a/inst/exdata/exam_questions.xlsx
+++ b/inst/exdata/exam_questions.xlsx
@@ -50,9 +50,6 @@
     <t>tf</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>mock</t>
   </si>
   <si>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>week1-2</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -401,7 +401,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:G15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -430,18 +430,18 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -450,30 +450,30 @@
         <v>2018</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
       <c r="E3">
         <v>2018</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -481,16 +481,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E4">
         <v>2018</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -498,50 +498,50 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>2018</v>
+      </c>
+      <c r="F5" t="s">
         <v>7</v>
       </c>
-      <c r="E5">
-        <v>2018</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
       <c r="E6">
         <v>2018</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
         <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -550,41 +550,41 @@
         <v>2018</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
       <c r="E8">
         <v>2018</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
         <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -593,30 +593,30 @@
         <v>2018</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>14</v>
       </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
       <c r="E10">
         <v>2018</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -624,16 +624,16 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E11">
         <v>2018</v>
       </c>
       <c r="G11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -641,50 +641,50 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <v>2018</v>
+      </c>
+      <c r="F12" t="s">
         <v>7</v>
       </c>
-      <c r="E12">
-        <v>2018</v>
-      </c>
-      <c r="F12" t="s">
-        <v>8</v>
-      </c>
       <c r="G12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
       <c r="E13">
         <v>2018</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
         <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -693,30 +693,30 @@
         <v>2018</v>
       </c>
       <c r="G14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>14</v>
       </c>
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
       <c r="E15">
         <v>2018</v>
       </c>
       <c r="F15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>